<commit_message>
Created opening Unicorn Browser, retrieving boys names.
</commit_message>
<xml_diff>
--- a/Data/Config.xlsx
+++ b/Data/Config.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23029"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24131"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\alexandra.veizu\Documents\Reframework_update_UiPath_Services\Data\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\fordern\Documents\UiPath\MedicoverTask\Data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9BE7DFF5-5AFC-4110-8461-609B0BDD5551}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5BE2646D-60AA-40AD-9024-15F5830152A6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Settings" sheetId="1" r:id="rId1"/>
@@ -22,7 +22,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="36" uniqueCount="32">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="40" uniqueCount="36">
   <si>
     <t>Name</t>
   </si>
@@ -90,19 +90,7 @@
     <t>Framework</t>
   </si>
   <si>
-    <t>ProcessABCQueue</t>
-    <phoneticPr fontId="2"/>
-  </si>
-  <si>
-    <t>Orchestrator queue Name. The value must match with the queue name defined on Orchestrator.</t>
-    <phoneticPr fontId="2"/>
-  </si>
-  <si>
     <t>Logging field which allows grouping of log data of two or more subprocesses under the same business process name</t>
-    <phoneticPr fontId="2"/>
-  </si>
-  <si>
-    <t>OrchestratorQueueName</t>
     <phoneticPr fontId="2"/>
   </si>
   <si>
@@ -123,12 +111,33 @@
   <si>
     <t>OrchestratorAssetFolder</t>
   </si>
+  <si>
+    <t>BoysSourceUrl</t>
+  </si>
+  <si>
+    <t>GirlsSourceUrl</t>
+  </si>
+  <si>
+    <t>UnicornNameUrl</t>
+  </si>
+  <si>
+    <t>https://www.rpasamples.com/unicornname</t>
+  </si>
+  <si>
+    <t>https://www.gov.pl/web/cyfryzacja/najpopularniejsze-imiona-dla-dziewczynek-2018-ranking-ogolnopolski</t>
+  </si>
+  <si>
+    <t>https://www.gov.pl/web/cyfryzacja/najpopularniejsze-imiona-dla-chlopcow-2018-ranking-ogolnopolski</t>
+  </si>
+  <si>
+    <t>NamesAmount</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="4">
+  <fonts count="5">
     <font>
       <sz val="11"/>
       <color rgb="FF000000"/>
@@ -152,6 +161,12 @@
       <name val="Calibri"/>
       <family val="2"/>
     </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color theme="10"/>
+      <name val="Calibri"/>
+    </font>
   </fonts>
   <fills count="2">
     <fill>
@@ -170,22 +185,24 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="1">
+  <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
   <cellXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="1" applyAlignment="1"/>
   </cellXfs>
-  <cellStyles count="1">
-    <cellStyle name="Normal" xfId="0" builtinId="0"/>
+  <cellStyles count="2">
+    <cellStyle name="Hiperłącze" xfId="1" builtinId="8"/>
+    <cellStyle name="Normalny" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
@@ -201,9 +218,9 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Motyw pakietu Office">
   <a:themeElements>
-    <a:clrScheme name="Office">
+    <a:clrScheme name="Pakiet Office">
       <a:dk1>
         <a:sysClr val="windowText" lastClr="000000"/>
       </a:dk1>
@@ -241,7 +258,7 @@
         <a:srgbClr val="954F72"/>
       </a:folHlink>
     </a:clrScheme>
-    <a:fontScheme name="Office">
+    <a:fontScheme name="Pakiet Office">
       <a:majorFont>
         <a:latin typeface="Calibri Light" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
@@ -347,7 +364,7 @@
         <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
-    <a:fmtScheme name="Office">
+    <a:fmtScheme name="Pakiet Office">
       <a:fillStyleLst>
         <a:solidFill>
           <a:schemeClr val="phClr"/>
@@ -497,10 +514,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:Z997"/>
+  <dimension ref="A1:Z996"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="C4" sqref="C4"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A9" sqref="A9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.42578125" defaultRowHeight="15" customHeight="1"/>
@@ -545,34 +562,52 @@
       <c r="Y1" s="1"/>
       <c r="Z1" s="1"/>
     </row>
-    <row r="2" spans="1:26" ht="14.25" customHeight="1">
-      <c r="A2" s="2" t="s">
-        <v>25</v>
-      </c>
-      <c r="B2" s="2" t="s">
+    <row r="2" spans="1:26" ht="14.25" customHeight="1"/>
+    <row r="3" spans="1:26" ht="30">
+      <c r="A3" t="s">
+        <v>20</v>
+      </c>
+      <c r="B3" t="s">
+        <v>21</v>
+      </c>
+      <c r="C3" s="3" t="s">
         <v>22</v>
       </c>
-      <c r="C2" s="2" t="s">
-        <v>23</v>
-      </c>
     </row>
-    <row r="3" spans="1:26" ht="14.25" customHeight="1"/>
-    <row r="4" spans="1:26" ht="30">
-      <c r="A4" t="s">
-        <v>20</v>
-      </c>
-      <c r="B4" t="s">
-        <v>21</v>
-      </c>
-      <c r="C4" s="4" t="s">
-        <v>24</v>
+    <row r="4" spans="1:26" ht="14.25" customHeight="1"/>
+    <row r="5" spans="1:26" ht="14.25" customHeight="1">
+      <c r="A5" t="s">
+        <v>29</v>
+      </c>
+      <c r="B5" s="4" t="s">
+        <v>34</v>
       </c>
     </row>
-    <row r="5" spans="1:26" ht="14.25" customHeight="1"/>
-    <row r="6" spans="1:26" ht="14.25" customHeight="1"/>
-    <row r="7" spans="1:26" ht="14.25" customHeight="1"/>
+    <row r="6" spans="1:26" ht="14.25" customHeight="1">
+      <c r="A6" t="s">
+        <v>30</v>
+      </c>
+      <c r="B6" s="4" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="7" spans="1:26" ht="14.25" customHeight="1">
+      <c r="A7" t="s">
+        <v>31</v>
+      </c>
+      <c r="B7" s="4" t="s">
+        <v>32</v>
+      </c>
+    </row>
     <row r="8" spans="1:26" ht="14.25" customHeight="1"/>
-    <row r="9" spans="1:26" ht="14.25" customHeight="1"/>
+    <row r="9" spans="1:26" ht="14.25" customHeight="1">
+      <c r="A9" t="s">
+        <v>35</v>
+      </c>
+      <c r="B9">
+        <v>10</v>
+      </c>
+    </row>
     <row r="10" spans="1:26" ht="14.25" customHeight="1"/>
     <row r="11" spans="1:26" ht="14.25" customHeight="1"/>
     <row r="12" spans="1:26" ht="14.25" customHeight="1"/>
@@ -1560,11 +1595,15 @@
     <row r="994" ht="14.25" customHeight="1"/>
     <row r="995" ht="14.25" customHeight="1"/>
     <row r="996" ht="14.25" customHeight="1"/>
-    <row r="997" ht="14.25" customHeight="1"/>
   </sheetData>
   <phoneticPr fontId="2"/>
+  <hyperlinks>
+    <hyperlink ref="B7" r:id="rId1" xr:uid="{98D1E264-65C8-400C-8269-7D89DDC128CD}"/>
+    <hyperlink ref="B6" r:id="rId2" xr:uid="{4EA6FA2C-9222-48F1-914D-B4E6CEE9F5F6}"/>
+    <hyperlink ref="B5" r:id="rId3" xr:uid="{63B52DE6-D6AD-4F14-A2E8-0B2594187729}"/>
+  </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId4"/>
 </worksheet>
 </file>
 
@@ -1623,8 +1662,8 @@
       <c r="B2">
         <v>0</v>
       </c>
-      <c r="C2" s="3" t="s">
-        <v>26</v>
+      <c r="C2" s="2" t="s">
+        <v>23</v>
       </c>
     </row>
     <row r="3" spans="1:26" ht="14.25" customHeight="1"/>
@@ -1648,7 +1687,7 @@
         <v>10</v>
       </c>
       <c r="C6" t="s">
-        <v>30</v>
+        <v>27</v>
       </c>
     </row>
     <row r="7" spans="1:26" ht="14.25" customHeight="1">
@@ -1670,7 +1709,7 @@
         <v>15</v>
       </c>
       <c r="C8" t="s">
-        <v>27</v>
+        <v>24</v>
       </c>
     </row>
     <row r="9" spans="1:26" ht="14.25" customHeight="1">
@@ -1681,7 +1720,7 @@
         <v>17</v>
       </c>
       <c r="C9" t="s">
-        <v>28</v>
+        <v>25</v>
       </c>
     </row>
     <row r="10" spans="1:26" ht="14.25" customHeight="1">
@@ -1692,7 +1731,7 @@
         <v>19</v>
       </c>
       <c r="C10" t="s">
-        <v>29</v>
+        <v>26</v>
       </c>
     </row>
     <row r="11" spans="1:26" ht="14.25" customHeight="1"/>
@@ -2682,8 +2721,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <dimension ref="A1:Z1000"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C2" sqref="A2:C2"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A25" sqref="A25"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.42578125" defaultRowHeight="15" customHeight="1"/>
@@ -2702,7 +2741,7 @@
         <v>2</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>31</v>
+        <v>28</v>
       </c>
       <c r="D1" s="1" t="s">
         <v>4</v>

</xml_diff>

<commit_message>
Completed retrieving girls names. Created transaction disposer.
</commit_message>
<xml_diff>
--- a/Data/Config.xlsx
+++ b/Data/Config.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\fordern\Documents\UiPath\MedicoverTask\Data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5BE2646D-60AA-40AD-9024-15F5830152A6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C86AFA18-7257-4411-AC07-E8AC620816A2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -517,7 +517,7 @@
   <dimension ref="A1:Z996"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A9" sqref="A9"/>
+      <selection activeCell="B16" sqref="B16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.42578125" defaultRowHeight="15" customHeight="1"/>
@@ -605,7 +605,7 @@
         <v>35</v>
       </c>
       <c r="B9">
-        <v>10</v>
+        <v>7</v>
       </c>
     </row>
     <row r="10" spans="1:26" ht="14.25" customHeight="1"/>

</xml_diff>

<commit_message>
Completed Process.xaml, TransactionItem converted from QueueItem to DataRow. Completed saving results to .xlsx spreadsheet.
</commit_message>
<xml_diff>
--- a/Data/Config.xlsx
+++ b/Data/Config.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\fordern\Documents\UiPath\MedicoverTask\Data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C86AFA18-7257-4411-AC07-E8AC620816A2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7CCF070C-9B1C-42A8-98DC-BBF4E6B53DAA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -22,7 +22,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="40" uniqueCount="36">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="53" uniqueCount="49">
   <si>
     <t>Name</t>
   </si>
@@ -131,6 +131,45 @@
   </si>
   <si>
     <t>NamesAmount</t>
+  </si>
+  <si>
+    <t>Source URL of boys names for processing.</t>
+  </si>
+  <si>
+    <t>Source URL of girls names for processing.</t>
+  </si>
+  <si>
+    <t>URL of Unicorn Name generator.</t>
+  </si>
+  <si>
+    <t>Determines how many names of each gender should be processed, starting from most popular.</t>
+  </si>
+  <si>
+    <t>OutputPath</t>
+  </si>
+  <si>
+    <t>InputPath</t>
+  </si>
+  <si>
+    <t>TemplateFileName</t>
+  </si>
+  <si>
+    <t>Filename of template excel spreadsheet.</t>
+  </si>
+  <si>
+    <t>Path for input files. Could be relative or full path.</t>
+  </si>
+  <si>
+    <t>Path for output files. Could be relative or full path.</t>
+  </si>
+  <si>
+    <t>template.xlsx</t>
+  </si>
+  <si>
+    <t>Data\Output</t>
+  </si>
+  <si>
+    <t>Data\Input</t>
   </si>
 </sst>
 </file>
@@ -517,7 +556,7 @@
   <dimension ref="A1:Z996"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B16" sqref="B16"/>
+      <selection activeCell="B13" sqref="B13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.42578125" defaultRowHeight="15" customHeight="1"/>
@@ -582,6 +621,9 @@
       <c r="B5" s="4" t="s">
         <v>34</v>
       </c>
+      <c r="C5" t="s">
+        <v>36</v>
+      </c>
     </row>
     <row r="6" spans="1:26" ht="14.25" customHeight="1">
       <c r="A6" t="s">
@@ -590,6 +632,9 @@
       <c r="B6" s="4" t="s">
         <v>33</v>
       </c>
+      <c r="C6" t="s">
+        <v>37</v>
+      </c>
     </row>
     <row r="7" spans="1:26" ht="14.25" customHeight="1">
       <c r="A7" t="s">
@@ -597,6 +642,9 @@
       </c>
       <c r="B7" s="4" t="s">
         <v>32</v>
+      </c>
+      <c r="C7" t="s">
+        <v>38</v>
       </c>
     </row>
     <row r="8" spans="1:26" ht="14.25" customHeight="1"/>
@@ -605,7 +653,10 @@
         <v>35</v>
       </c>
       <c r="B9">
-        <v>7</v>
+        <v>10</v>
+      </c>
+      <c r="C9" t="s">
+        <v>39</v>
       </c>
     </row>
     <row r="10" spans="1:26" ht="14.25" customHeight="1"/>
@@ -1609,9 +1660,11 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
-  <dimension ref="A1:Z987"/>
+  <dimension ref="A1:Z989"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="C6" sqref="C6"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.42578125" defaultRowHeight="15" customHeight="1"/>
   <cols>
@@ -1660,7 +1713,7 @@
         <v>5</v>
       </c>
       <c r="B2">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="C2" s="2" t="s">
         <v>23</v>
@@ -1735,10 +1788,42 @@
       </c>
     </row>
     <row r="11" spans="1:26" ht="14.25" customHeight="1"/>
-    <row r="12" spans="1:26" ht="14.25" customHeight="1"/>
-    <row r="13" spans="1:26" ht="14.25" customHeight="1"/>
-    <row r="14" spans="1:26" ht="14.25" customHeight="1"/>
-    <row r="15" spans="1:26" ht="14.25" customHeight="1"/>
+    <row r="12" spans="1:26" ht="14.25" customHeight="1">
+      <c r="A12" t="s">
+        <v>41</v>
+      </c>
+      <c r="B12" t="s">
+        <v>48</v>
+      </c>
+      <c r="C12" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="13" spans="1:26" ht="14.25" customHeight="1">
+      <c r="A13" t="s">
+        <v>42</v>
+      </c>
+      <c r="B13" t="s">
+        <v>46</v>
+      </c>
+      <c r="C13" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="14" spans="1:26" ht="14.25" customHeight="1">
+      <c r="A14" t="s">
+        <v>40</v>
+      </c>
+      <c r="B14" t="s">
+        <v>47</v>
+      </c>
+      <c r="C14" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="15" spans="1:26" ht="14.25" customHeight="1">
+      <c r="C15" s="2"/>
+    </row>
     <row r="16" spans="1:26" ht="14.25" customHeight="1"/>
     <row r="17" ht="14.25" customHeight="1"/>
     <row r="18" ht="14.25" customHeight="1"/>
@@ -2711,6 +2796,8 @@
     <row r="985" ht="14.25" customHeight="1"/>
     <row r="986" ht="14.25" customHeight="1"/>
     <row r="987" ht="14.25" customHeight="1"/>
+    <row r="988" ht="14.25" customHeight="1"/>
+    <row r="989" ht="14.25" customHeight="1"/>
   </sheetData>
   <phoneticPr fontId="2"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
Moved workflow between directories.
</commit_message>
<xml_diff>
--- a/Data/Config.xlsx
+++ b/Data/Config.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\fordern\Documents\UiPath\MedicoverTask\Data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7CCF070C-9B1C-42A8-98DC-BBF4E6B53DAA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{28AA13AF-1DC8-4E2C-B4AB-967458849C23}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-135" yWindow="-135" windowWidth="29070" windowHeight="15870" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Settings" sheetId="1" r:id="rId1"/>
@@ -124,52 +124,52 @@
     <t>https://www.rpasamples.com/unicornname</t>
   </si>
   <si>
+    <t>NamesAmount</t>
+  </si>
+  <si>
+    <t>Source URL of boys names for processing.</t>
+  </si>
+  <si>
+    <t>Source URL of girls names for processing.</t>
+  </si>
+  <si>
+    <t>URL of Unicorn Name generator.</t>
+  </si>
+  <si>
+    <t>Determines how many names of each gender should be processed, starting from most popular.</t>
+  </si>
+  <si>
+    <t>OutputPath</t>
+  </si>
+  <si>
+    <t>InputPath</t>
+  </si>
+  <si>
+    <t>TemplateFileName</t>
+  </si>
+  <si>
+    <t>Filename of template excel spreadsheet.</t>
+  </si>
+  <si>
+    <t>Path for input files. Could be relative or full path.</t>
+  </si>
+  <si>
+    <t>Path for output files. Could be relative or full path.</t>
+  </si>
+  <si>
+    <t>template.xlsx</t>
+  </si>
+  <si>
+    <t>Data\Output</t>
+  </si>
+  <si>
+    <t>Data\Input</t>
+  </si>
+  <si>
     <t>https://www.gov.pl/web/cyfryzacja/najpopularniejsze-imiona-dla-dziewczynek-2018-ranking-ogolnopolski</t>
   </si>
   <si>
     <t>https://www.gov.pl/web/cyfryzacja/najpopularniejsze-imiona-dla-chlopcow-2018-ranking-ogolnopolski</t>
-  </si>
-  <si>
-    <t>NamesAmount</t>
-  </si>
-  <si>
-    <t>Source URL of boys names for processing.</t>
-  </si>
-  <si>
-    <t>Source URL of girls names for processing.</t>
-  </si>
-  <si>
-    <t>URL of Unicorn Name generator.</t>
-  </si>
-  <si>
-    <t>Determines how many names of each gender should be processed, starting from most popular.</t>
-  </si>
-  <si>
-    <t>OutputPath</t>
-  </si>
-  <si>
-    <t>InputPath</t>
-  </si>
-  <si>
-    <t>TemplateFileName</t>
-  </si>
-  <si>
-    <t>Filename of template excel spreadsheet.</t>
-  </si>
-  <si>
-    <t>Path for input files. Could be relative or full path.</t>
-  </si>
-  <si>
-    <t>Path for output files. Could be relative or full path.</t>
-  </si>
-  <si>
-    <t>template.xlsx</t>
-  </si>
-  <si>
-    <t>Data\Output</t>
-  </si>
-  <si>
-    <t>Data\Input</t>
   </si>
 </sst>
 </file>
@@ -556,7 +556,7 @@
   <dimension ref="A1:Z996"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B13" sqref="B13"/>
+      <selection activeCell="B5" sqref="B5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.42578125" defaultRowHeight="15" customHeight="1"/>
@@ -619,10 +619,10 @@
         <v>29</v>
       </c>
       <c r="B5" s="4" t="s">
+        <v>48</v>
+      </c>
+      <c r="C5" t="s">
         <v>34</v>
-      </c>
-      <c r="C5" t="s">
-        <v>36</v>
       </c>
     </row>
     <row r="6" spans="1:26" ht="14.25" customHeight="1">
@@ -630,10 +630,10 @@
         <v>30</v>
       </c>
       <c r="B6" s="4" t="s">
-        <v>33</v>
+        <v>47</v>
       </c>
       <c r="C6" t="s">
-        <v>37</v>
+        <v>35</v>
       </c>
     </row>
     <row r="7" spans="1:26" ht="14.25" customHeight="1">
@@ -644,19 +644,19 @@
         <v>32</v>
       </c>
       <c r="C7" t="s">
-        <v>38</v>
+        <v>36</v>
       </c>
     </row>
     <row r="8" spans="1:26" ht="14.25" customHeight="1"/>
     <row r="9" spans="1:26" ht="14.25" customHeight="1">
       <c r="A9" t="s">
-        <v>35</v>
+        <v>33</v>
       </c>
       <c r="B9">
         <v>10</v>
       </c>
       <c r="C9" t="s">
-        <v>39</v>
+        <v>37</v>
       </c>
     </row>
     <row r="10" spans="1:26" ht="14.25" customHeight="1"/>
@@ -1650,11 +1650,9 @@
   <phoneticPr fontId="2"/>
   <hyperlinks>
     <hyperlink ref="B7" r:id="rId1" xr:uid="{98D1E264-65C8-400C-8269-7D89DDC128CD}"/>
-    <hyperlink ref="B6" r:id="rId2" xr:uid="{4EA6FA2C-9222-48F1-914D-B4E6CEE9F5F6}"/>
-    <hyperlink ref="B5" r:id="rId3" xr:uid="{63B52DE6-D6AD-4F14-A2E8-0B2594187729}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" orientation="portrait" r:id="rId4"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId2"/>
 </worksheet>
 </file>
 
@@ -1663,7 +1661,7 @@
   <dimension ref="A1:Z989"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="C6" sqref="C6"/>
+      <selection activeCell="C14" sqref="C14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.42578125" defaultRowHeight="15" customHeight="1"/>
@@ -1790,35 +1788,35 @@
     <row r="11" spans="1:26" ht="14.25" customHeight="1"/>
     <row r="12" spans="1:26" ht="14.25" customHeight="1">
       <c r="A12" t="s">
-        <v>41</v>
+        <v>39</v>
       </c>
       <c r="B12" t="s">
-        <v>48</v>
+        <v>46</v>
       </c>
       <c r="C12" t="s">
-        <v>44</v>
+        <v>42</v>
       </c>
     </row>
     <row r="13" spans="1:26" ht="14.25" customHeight="1">
       <c r="A13" t="s">
-        <v>42</v>
+        <v>40</v>
       </c>
       <c r="B13" t="s">
-        <v>46</v>
+        <v>44</v>
       </c>
       <c r="C13" t="s">
-        <v>43</v>
+        <v>41</v>
       </c>
     </row>
     <row r="14" spans="1:26" ht="14.25" customHeight="1">
       <c r="A14" t="s">
-        <v>40</v>
+        <v>38</v>
       </c>
       <c r="B14" t="s">
-        <v>47</v>
+        <v>45</v>
       </c>
       <c r="C14" t="s">
-        <v>45</v>
+        <v>43</v>
       </c>
     </row>
     <row r="15" spans="1:26" ht="14.25" customHeight="1">

</xml_diff>